<commit_message>
Fixing the dataset analysis sheet for the output order from Casaletto as well as adding a summary sheet.
</commit_message>
<xml_diff>
--- a/Labs/Lab1/CS286 - Lab #1 Dataset Analysis.xlsx
+++ b/Labs/Lab1/CS286 - Lab #1 Dataset Analysis.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Output" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="iris_data" localSheetId="0">Sheet1!$A$1:$E$150</definedName>
+    <definedName name="iris_data" localSheetId="0">'Raw Data'!$A$1:$E$150</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>Min</t>
   </si>
@@ -51,14 +50,34 @@
   <si>
     <t>Petal Length</t>
   </si>
+  <si>
+    <t>Sepal Width</t>
+  </si>
+  <si>
+    <t>Petal Width</t>
+  </si>
+  <si>
+    <t>Final Output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -259,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -300,6 +319,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,19 +699,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H2" s="14">
-        <f>MIN($A$1:$A$50)</f>
-        <v>4.3</v>
+        <f>MIN($B$1:$B$50)</f>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I2" s="14">
-        <f>MAX($A$1:$A$50)</f>
-        <v>5.8</v>
+        <f>MAX($B$1:$B$50)</f>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J2" s="15">
-        <f>AVERAGE($A$1:$A$50)</f>
-        <v>5.0059999999999993</v>
+        <f>AVERAGE($B$1:$B$50)</f>
+        <v>3.4280000000000008</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -696,16 +734,16 @@
         <v>3</v>
       </c>
       <c r="H3" s="14">
-        <f>MIN($B$1:$B$50)</f>
-        <v>2.2999999999999998</v>
+        <f>MIN($A$1:$A$50)</f>
+        <v>4.3</v>
       </c>
       <c r="I3" s="14">
-        <f>MAX($B$1:$B$50)</f>
-        <v>4.4000000000000004</v>
+        <f>MAX($A$1:$A$50)</f>
+        <v>5.8</v>
       </c>
       <c r="J3" s="15">
-        <f>AVERAGE($B$1:$B$50)</f>
-        <v>3.4280000000000008</v>
+        <f>AVERAGE($A$1:$A$50)</f>
+        <v>5.0059999999999993</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -725,19 +763,19 @@
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4" s="14">
-        <f>MIN($C$1:$C$50)</f>
-        <v>1</v>
+        <f>MIN($D$1:$D$50)</f>
+        <v>0.1</v>
       </c>
       <c r="I4" s="14">
-        <f>MAX($C$1:$C$50)</f>
-        <v>1.9</v>
+        <f>MAX($D$1:$D$50)</f>
+        <v>0.6</v>
       </c>
       <c r="J4" s="15">
-        <f>AVERAGE($C$1:$C$50)</f>
-        <v>1.4620000000000002</v>
+        <f>AVERAGE($D$1:$D$50)</f>
+        <v>0.24599999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -760,16 +798,16 @@
         <v>4</v>
       </c>
       <c r="H5" s="17">
-        <f>MIN($D$1:$D$50)</f>
-        <v>0.1</v>
+        <f>MIN($C$1:$C$50)</f>
+        <v>1</v>
       </c>
       <c r="I5" s="17">
-        <f>MAX($D$1:$D$50)</f>
-        <v>0.6</v>
+        <f>MAX($C$1:$C$50)</f>
+        <v>1.9</v>
       </c>
       <c r="J5" s="18">
-        <f>AVERAGE($D$1:$D$50)</f>
-        <v>0.24599999999999991</v>
+        <f>AVERAGE($C$1:$C$50)</f>
+        <v>1.4620000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1581,19 +1619,19 @@
         <v>1</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H52" s="14">
-        <f>MIN($A$51:$A$100)</f>
-        <v>4.9000000000000004</v>
+        <f>MIN($B$51:$B$100)</f>
+        <v>2</v>
       </c>
       <c r="I52" s="14">
-        <f>MAX($A$51:$A$100)</f>
-        <v>7</v>
+        <f>MAX($B$51:$B$100)</f>
+        <v>3.4</v>
       </c>
       <c r="J52" s="15">
-        <f>AVERAGE($A$51:$A$100)</f>
-        <v>5.9359999999999999</v>
+        <f>AVERAGE($B$51:$B$100)</f>
+        <v>2.7700000000000005</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -1616,16 +1654,16 @@
         <v>3</v>
       </c>
       <c r="H53" s="14">
-        <f>MIN($B$51:$B$100)</f>
-        <v>2</v>
+        <f>MIN($A$51:$A$100)</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I53" s="14">
-        <f>MAX($B$51:$B$100)</f>
-        <v>3.4</v>
+        <f>MAX($A$51:$A$100)</f>
+        <v>7</v>
       </c>
       <c r="J53" s="15">
-        <f>AVERAGE($B$51:$B$100)</f>
-        <v>2.7700000000000005</v>
+        <f>AVERAGE($A$51:$A$100)</f>
+        <v>5.9359999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -1645,19 +1683,19 @@
         <v>1</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H54" s="14">
-        <f>MIN($C$51:$C$100)</f>
-        <v>3</v>
+        <f>MIN($D$51:$D$100)</f>
+        <v>1</v>
       </c>
       <c r="I54" s="14">
-        <f>MAX($C$51:$C$100)</f>
-        <v>5.0999999999999996</v>
+        <f>MAX($D$51:$D$100)</f>
+        <v>1.8</v>
       </c>
       <c r="J54" s="15">
-        <f>AVERAGE($C$51:$C$100)</f>
-        <v>4.26</v>
+        <f>AVERAGE($D$51:$D$100)</f>
+        <v>1.3259999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1680,16 +1718,16 @@
         <v>4</v>
       </c>
       <c r="H55" s="17">
-        <f>MIN($D$51:$D$100)</f>
-        <v>1</v>
+        <f>MIN($C$51:$C$100)</f>
+        <v>3</v>
       </c>
       <c r="I55" s="17">
-        <f>MAX($D$51:$D$100)</f>
-        <v>1.8</v>
+        <f>MAX($C$51:$C$100)</f>
+        <v>5.0999999999999996</v>
       </c>
       <c r="J55" s="18">
-        <f>AVERAGE($D$51:$D$100)</f>
-        <v>1.3259999999999998</v>
+        <f>AVERAGE($C$51:$C$100)</f>
+        <v>4.26</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2501,19 +2539,19 @@
         <v>2</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H102" s="14">
-        <f>MIN($A$101:$A$150)</f>
-        <v>4.9000000000000004</v>
+        <f>MIN($B$101:$B$150)</f>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I102" s="14">
-        <f>MAX($A$101:$A$150)</f>
-        <v>7.9</v>
+        <f>MAX($B$101:$B$150)</f>
+        <v>3.8</v>
       </c>
       <c r="J102" s="15">
-        <f>AVERAGE($A$101:$A$150)</f>
-        <v>6.5879999999999983</v>
+        <f>AVERAGE($B$101:$B$150)</f>
+        <v>2.9739999999999998</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -2536,16 +2574,16 @@
         <v>3</v>
       </c>
       <c r="H103" s="14">
-        <f>MIN($B$101:$B$150)</f>
-        <v>2.2000000000000002</v>
+        <f>MIN($A$101:$A$150)</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I103" s="14">
-        <f>MAX($B$101:$B$150)</f>
-        <v>3.8</v>
+        <f>MAX($A$101:$A$150)</f>
+        <v>7.9</v>
       </c>
       <c r="J103" s="15">
-        <f>AVERAGE($B$101:$B$150)</f>
-        <v>2.9739999999999998</v>
+        <f>AVERAGE($A$101:$A$150)</f>
+        <v>6.5879999999999983</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -2565,19 +2603,19 @@
         <v>2</v>
       </c>
       <c r="G104" s="13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H104" s="14">
-        <f>MIN($C$101:$C$150)</f>
-        <v>4.5</v>
+        <f>MIN($D$101:$D$150)</f>
+        <v>1.4</v>
       </c>
       <c r="I104" s="14">
-        <f>MAX($C$101:$C$150)</f>
-        <v>6.9</v>
+        <f>MAX($D$101:$D$150)</f>
+        <v>2.5</v>
       </c>
       <c r="J104" s="15">
-        <f>AVERAGE($C$101:$C$150)</f>
-        <v>5.5519999999999996</v>
+        <f>AVERAGE($D$101:$D$150)</f>
+        <v>2.0259999999999998</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2600,16 +2638,16 @@
         <v>4</v>
       </c>
       <c r="H105" s="17">
-        <f>MIN($D$101:$D$150)</f>
-        <v>1.4</v>
+        <f>MIN($C$101:$C$150)</f>
+        <v>4.5</v>
       </c>
       <c r="I105" s="17">
-        <f>MAX($D$101:$D$150)</f>
-        <v>2.5</v>
+        <f>MAX($C$101:$C$150)</f>
+        <v>6.9</v>
       </c>
       <c r="J105" s="18">
-        <f>AVERAGE($D$101:$D$150)</f>
-        <v>2.0259999999999998</v>
+        <f>AVERAGE($C$101:$C$150)</f>
+        <v>5.5519999999999996</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3386,24 +3424,179 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>0</v>
+      </c>
+      <c r="B3" s="25">
+        <f>'Raw Data'!$H$2</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C3" s="25">
+        <f>'Raw Data'!$I$2</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D3" s="11">
+        <f>'Raw Data'!$J$2</f>
+        <v>3.4280000000000008</v>
+      </c>
+      <c r="E3" s="25">
+        <f>'Raw Data'!$H$3</f>
+        <v>4.3</v>
+      </c>
+      <c r="F3" s="25">
+        <f>'Raw Data'!$I$3</f>
+        <v>5.8</v>
+      </c>
+      <c r="G3" s="11">
+        <f>'Raw Data'!$J$3</f>
+        <v>5.0059999999999993</v>
+      </c>
+      <c r="H3" s="25">
+        <f>'Raw Data'!$H$4</f>
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="25">
+        <f>'Raw Data'!$I$4</f>
+        <v>0.6</v>
+      </c>
+      <c r="J3" s="11">
+        <f>'Raw Data'!$J$4</f>
+        <v>0.24599999999999991</v>
+      </c>
+      <c r="K3" s="25">
+        <f>'Raw Data'!$H$5</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="25">
+        <f>'Raw Data'!$I$5</f>
+        <v>1.9</v>
+      </c>
+      <c r="M3" s="12">
+        <f>'Raw Data'!$J$5</f>
+        <v>1.4620000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26">
+        <f>'Raw Data'!$H$52</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="26">
+        <f>'Raw Data'!$I$52</f>
+        <v>3.4</v>
+      </c>
+      <c r="D4" s="14">
+        <f>'Raw Data'!$J$52</f>
+        <v>2.7700000000000005</v>
+      </c>
+      <c r="E4" s="26">
+        <f>'Raw Data'!$H$53</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F4" s="26">
+        <f>'Raw Data'!$I$53</f>
+        <v>7</v>
+      </c>
+      <c r="G4" s="14">
+        <f>'Raw Data'!$J$53</f>
+        <v>5.9359999999999999</v>
+      </c>
+      <c r="H4" s="26">
+        <f>'Raw Data'!$H$54</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="26">
+        <f>'Raw Data'!$I$54</f>
+        <v>1.8</v>
+      </c>
+      <c r="J4" s="14">
+        <f>'Raw Data'!$J$54</f>
+        <v>1.3259999999999998</v>
+      </c>
+      <c r="K4" s="26">
+        <f>'Raw Data'!$H$55</f>
+        <v>3</v>
+      </c>
+      <c r="L4" s="26">
+        <f>'Raw Data'!$I$55</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M4" s="15">
+        <f>'Raw Data'!$J$55</f>
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27">
+        <f>'Raw Data'!$H$102</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C5" s="27">
+        <f>'Raw Data'!$I$102</f>
+        <v>3.8</v>
+      </c>
+      <c r="D5" s="17">
+        <f>'Raw Data'!$J$102</f>
+        <v>2.9739999999999998</v>
+      </c>
+      <c r="E5" s="27">
+        <f>'Raw Data'!$H$103</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F5" s="27">
+        <f>'Raw Data'!$I$103</f>
+        <v>7.9</v>
+      </c>
+      <c r="G5" s="17">
+        <f>'Raw Data'!$J$103</f>
+        <v>6.5879999999999983</v>
+      </c>
+      <c r="H5" s="27">
+        <f>'Raw Data'!$H$104</f>
+        <v>1.4</v>
+      </c>
+      <c r="I5" s="27">
+        <f>'Raw Data'!$I$104</f>
+        <v>2.5</v>
+      </c>
+      <c r="J5" s="17">
+        <f>'Raw Data'!$J$104</f>
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="K5" s="27">
+        <f>'Raw Data'!$H$105</f>
+        <v>4.5</v>
+      </c>
+      <c r="L5" s="27">
+        <f>'Raw Data'!$I$105</f>
+        <v>6.9</v>
+      </c>
+      <c r="M5" s="18">
+        <f>'Raw Data'!$J$105</f>
+        <v>5.5519999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>